<commit_message>
Update on the excle file content
</commit_message>
<xml_diff>
--- a/Output/cleaned_column_names_2.xlsx
+++ b/Output/cleaned_column_names_2.xlsx
@@ -1213,189 +1213,189 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>rshp_to_head</t>
+          <t>female_int_eligibility</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>slept_llin_net</t>
+          <t>year_of birth</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>blood_smear_bar_code</t>
+          <t>individual_file_pregnancy_status</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>malariae_present</t>
+          <t>brand_of_net</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>line_number_of_person_slept_in_net</t>
+          <t>century_day_code_of_birth</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>date_measured_day</t>
+          <t>month_of_data_collection</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>day_of_data_collection</t>
+          <t>hemoglobin_level_adjusted_for_altitude_g_dl</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>fieldworker_measurer_code</t>
+          <t>na_read_consent_statement_for_malaria</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>completeleness_of_hc32_info</t>
+          <t>insecticide_treated_net</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>cmc_date_of_birth</t>
+          <t>childs_age_in_days</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>ovale_present</t>
+          <t>read_consent_statement_hemoglobin</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>corr_age</t>
+          <t>index_to_household_schedule_hmhidx</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>number_of_persons_slept_under_net</t>
+          <t>month_of_birth</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>female_int_eligibility</t>
+          <t>mothers_line_number</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>brand_of_net</t>
+          <t>malariae_present</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>year_of birth</t>
+          <t>net_observed_by_interviewer</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>caretaker_line_number</t>
+          <t>rshp_to_head</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>read_consent_statement_hemoglobin</t>
+          <t>date_measured_day</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>sex</t>
+          <t>line_number_of_person_slept_in_net</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>bed_net_type</t>
+          <t>net_from_antenatal_immunization_visit</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>months_ago_net_obtained</t>
+          <t>childs_age_in_months</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>individual_file_pregnancy_status</t>
+          <t>sex_of_member</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>century_day_code_of_birth</t>
+          <t>line_number_of_parent_caretaker</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>malaria_measurement_result</t>
+          <t>net_design_no</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>hemoglobin_level_g_dl</t>
+          <t>slept_under_net</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>mosquito_bed_net_designation_number</t>
+          <t>corr_age</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>slept_last_night</t>
+          <t>flag_age</t>
         </is>
       </c>
     </row>
@@ -1409,259 +1409,259 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>vivax_present</t>
+          <t>date_measured_month</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>day_of_birth</t>
+          <t>date_measured_year</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>mothers_line_number</t>
+          <t>caretaker_line_number</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>usual_resident</t>
+          <t>vivax_present</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>century_day_code_of_measurement</t>
+          <t>ovale_present</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>sex_of_member</t>
+          <t>sex</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>net_from_antenatal_immunization_visit</t>
+          <t>age_of_member</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>index_to_household_schedule_hmhidx</t>
+          <t>anemia_level</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>childs_age_in_days_country_specific</t>
+          <t>malaria_measurement_result</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>rapid_test_result</t>
+          <t>day_of_birth</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>slept_under_net</t>
+          <t>day_of_data_collection</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>na_read_consent_statement_for_malaria</t>
+          <t>line_number</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>insecticide_treated_net</t>
+          <t>childs_age_in_months_country_specific</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>result_of_measurement_hemoglobin</t>
+          <t>number_of_persons_slept_under_net</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>date_measured_month</t>
+          <t>cmc_date_of_birth</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>age_of_member</t>
+          <t>months_ago_net_obtained</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>month_of_birth</t>
+          <t>hemoglobin_level_g_dl</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>childs_age_in_months_country_specific_hml16a</t>
+          <t>child_age_in_months</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>line_number_of_parent_caretaker</t>
+          <t>century_day_code_of_measurement</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>net_observed_by_interviewer</t>
+          <t>fieldworker_measurer_code</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>children_hemoglobin_elig</t>
+          <t>mosquito_bed_net_designation_number</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>flag_age</t>
+          <t>blood_smear_bar_code</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>date_measured_year</t>
+          <t>bed_net_type</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>childs_age_in_months</t>
+          <t>index_to_household_schedule_hc0</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>net_design_no</t>
+          <t>childs_age_in_days_country_specific</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>child_age_in_months</t>
+          <t>someone_slept_under_net_last_night</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>index_to_household_schedule_hc0</t>
+          <t>childs_age_in_months_country_specific_hml16a</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>someone_slept_under_net_last_night</t>
+          <t>year_of_data_collection</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>month_of_data_collection</t>
+          <t>children_hemoglobin_elig</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>year_of_data_collection</t>
+          <t>falciparum_present</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>childs_age_in_days</t>
+          <t>result_of_measurement_hemoglobin</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>anemia_level</t>
+          <t>usual_resident</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>hemoglobin_level_adjusted_for_altitude_g_dl</t>
+          <t>slept_last_night</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>falciparum_present</t>
+          <t>slept_llin_net</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>line_number</t>
+          <t>completeleness_of_hc32_info</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>fieldworker_malaria_measurer_code</t>
+          <t>rapid_test_result</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>childs_age_in_months_country_specific</t>
+          <t>fieldworker_malaria_measurer_code</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update made to the jupyter notebook modelling and evaluation
</commit_message>
<xml_diff>
--- a/Output/cleaned_column_names_2.xlsx
+++ b/Output/cleaned_column_names_2.xlsx
@@ -1213,14 +1213,14 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>completeleness_of_hc32_info</t>
+          <t>final_blood_smear_test</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>date_measured_month</t>
+          <t>mothers_line_number</t>
         </is>
       </c>
     </row>
@@ -1234,238 +1234,238 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>vivax_present</t>
+          <t>malariae_present</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>rapid_test_result</t>
+          <t>blood_smear_bar_code</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>rshp_to_head</t>
+          <t>line_number</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>day_of_birth</t>
+          <t>read_consent_statement_hemoglobin</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>childs_age_in_months_country_specific</t>
+          <t>ovale_present</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>childs_age_in_months</t>
+          <t>someone_slept_under_net_last_night</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>net_from_antenatal_immunization_visit</t>
+          <t>day_of_birth</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>slept_under_net</t>
+          <t>childs_age_in_months</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>childs_age_in_months_country_specific_hml16a</t>
+          <t>net_design_no</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>individual_file_pregnancy_status</t>
+          <t>na_read_consent_statement_for_malaria</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>sex</t>
+          <t>falciparum_present</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>month_of_birth</t>
+          <t>cmc_date_of_birth</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>malariae_present</t>
+          <t>month_of_data_collection</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>year_of_data_collection</t>
+          <t>usual_resident</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>fieldworker_measurer_code</t>
+          <t>day_of_data_collection</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>mothers_line_number</t>
+          <t>malaria_measurement_result</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>cmc_date_of_birth</t>
+          <t>children_hemoglobin_elig</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>line_number</t>
+          <t>hemoglobin_level_g_dl</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>date_measured_year</t>
+          <t>childs_age_in_months_country_specific</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>usual_resident</t>
+          <t>childs_age_in_days_country_specific</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>hemoglobin_level_adjusted_for_altitude_g_dl</t>
+          <t>century_day_code_of_birth</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>slept_llin_net</t>
+          <t>bed_net_type</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>slept_last_night</t>
+          <t>child_age_in_months</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>caretaker_line_number</t>
+          <t>index_to_household_schedule_hc0</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>century_day_code_of_birth</t>
+          <t>childs_age_in_months_country_specific_hml16a</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>final_blood_smear_test</t>
+          <t>slept_llin_net</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>line_number_of_person_slept_in_net</t>
+          <t>corr_age</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>mosquito_bed_net_designation_number</t>
+          <t>result_of_measurement_hemoglobin</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>blood_smear_bar_code</t>
+          <t>vivax_present</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>net_design_no</t>
+          <t>year_of_data_collection</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>falciparum_present</t>
+          <t>date_measured_day</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>number_of_persons_slept_under_net</t>
+          <t>individual_file_pregnancy_status</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>hemoglobin_level_g_dl</t>
+          <t>month_of_birth</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>date_measured_day</t>
+          <t>line_number_of_parent_caretaker</t>
         </is>
       </c>
     </row>
@@ -1479,189 +1479,189 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>child_age_in_months</t>
+          <t>slept_last_night</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>brand_of_net</t>
+          <t>net_from_antenatal_immunization_visit</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>ovale_present</t>
+          <t>female_int_eligibility</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>index_to_household_schedule_hc0</t>
+          <t>number_of_persons_slept_under_net</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>month_of_data_collection</t>
+          <t>sex</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>year_of birth</t>
+          <t>insecticide_treated_net</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>corr_age</t>
+          <t>flag_age</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>children_hemoglobin_elig</t>
+          <t>rapid_test_result</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>childs_age_in_days</t>
+          <t>date_measured_month</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>day_of_data_collection</t>
+          <t>slept_under_net</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>index_to_household_schedule_hmhidx</t>
+          <t>childs_age_in_days</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>childs_age_in_days_country_specific</t>
+          <t>completeleness_of_hc32_info</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>anemia_level</t>
+          <t>caretaker_line_number</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>someone_slept_under_net_last_night</t>
+          <t>index_to_household_schedule_hmhidx</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>fieldworker_malaria_measurer_code</t>
+          <t>fieldworker_measurer_code</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>century_day_code_of_measurement</t>
+          <t>hemoglobin_level_adjusted_for_altitude_g_dl</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>malaria_measurement_result</t>
+          <t>year_of birth</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>net_observed_by_interviewer</t>
+          <t>anemia_level</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>result_of_measurement_hemoglobin</t>
+          <t>century_day_code_of_measurement</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>insecticide_treated_net</t>
+          <t>rshp_to_head</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>flag_age</t>
+          <t>date_measured_year</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>age_of_member</t>
+          <t>mosquito_bed_net_designation_number</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>bed_net_type</t>
+          <t>line_number_of_person_slept_in_net</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>female_int_eligibility</t>
+          <t>net_observed_by_interviewer</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>na_read_consent_statement_for_malaria</t>
+          <t>brand_of_net</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>line_number_of_parent_caretaker</t>
+          <t>age_of_member</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>read_consent_statement_hemoglobin</t>
+          <t>fieldworker_malaria_measurer_code</t>
         </is>
       </c>
     </row>

</xml_diff>